<commit_message>
modified:   01_Project management/6 Stakeholders management/COS-stockholder Register.xlsx 	modified:   03_Design/33_Design Documentation/System Analysis and Design_V1.3.docx 	modified:   06_Maintenance/61_Installation Manual/Installation Manual.docx 	modified:   07_Training/User Manual_ V1.0.docx 	modified:   08_Closing/Charity T1  handbook.docx 	modified:   08_Closing/Client Acceptance.doc 	modified:   09_Marketing/Charity T1  handbook.docx 	modified:   README.md
</commit_message>
<xml_diff>
--- a/01_Project management/6 Stakeholders management/COS-stockholder Register.xlsx
+++ b/01_Project management/6 Stakeholders management/COS-stockholder Register.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\项目文档\01_PM\6 Stakeholders management\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Downloads\0_Project document-20210505T043744Z-001\CharityOnlineStore\01_Project management\6 Stakeholders management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6508A522-87DA-4689-B7BF-11E8D95796E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B96B3D78-2DF4-4301-8B7C-B0FCC2AF304C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21720" yWindow="-1875" windowWidth="21840" windowHeight="13140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
   <si>
     <t>Client</t>
   </si>
@@ -115,12 +115,6 @@
     <t xml:space="preserve">Impact on project </t>
   </si>
   <si>
-    <t>PM</t>
-  </si>
-  <si>
-    <t>Developer</t>
-  </si>
-  <si>
     <t>Update Date</t>
   </si>
   <si>
@@ -134,6 +128,9 @@
   </si>
   <si>
     <t>Initial</t>
+  </si>
+  <si>
+    <t>Team member</t>
   </si>
 </sst>
 </file>
@@ -475,6 +472,21 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -495,21 +507,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -861,7 +858,7 @@
   <dimension ref="D9:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18:D19"/>
+      <selection activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
@@ -875,51 +872,51 @@
   </cols>
   <sheetData>
     <row r="9" spans="4:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="4:7" ht="31.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D10" s="21" t="s">
+    <row r="10" spans="4:7" ht="16" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D10" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="F10" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="E10" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="F10" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="G10" s="22" t="s">
+      <c r="G10" s="15" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="11" spans="4:7" ht="16" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D11" s="23">
+      <c r="D11" s="16">
         <v>43910</v>
       </c>
-      <c r="E11" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="F11" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="G11" s="24" t="s">
+      <c r="E11" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="G11" s="17" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="12" spans="4:7" ht="16" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D12" s="25"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="24"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17"/>
     </row>
     <row r="13" spans="4:7" ht="16" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D13" s="25"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="24"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
     </row>
     <row r="14" spans="4:7" ht="16" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D14" s="25"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="24"/>
-      <c r="G14" s="24"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -931,7 +928,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD22"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
@@ -948,29 +945,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="17"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="19" t="s">
+      <c r="C1" s="22"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="F1" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="19" t="s">
+      <c r="G1" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="19" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="20"/>
+      <c r="A2" s="25"/>
       <c r="B2" s="8" t="s">
         <v>3</v>
       </c>
@@ -980,10 +977,10 @@
       <c r="D2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="15"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="20"/>
     </row>
     <row r="3" spans="1:8" ht="47" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
@@ -1055,7 +1052,7 @@
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="6" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="F6" s="11" t="s">
         <v>23</v>
@@ -1075,7 +1072,7 @@
       </c>
       <c r="D7" s="6"/>
       <c r="E7" s="6" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="F7" s="13" t="s">
         <v>22</v>

</xml_diff>